<commit_message>
chore: excel file changed
</commit_message>
<xml_diff>
--- a/data/wrong.xlsx
+++ b/data/wrong.xlsx
@@ -14,153 +14,150 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>valor</t>
-  </si>
-  <si>
-    <t>produto</t>
-  </si>
-  <si>
-    <t>quantidade</t>
-  </si>
-  <si>
-    <t>categoria</t>
+    <t>date</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Produto A</t>
-  </si>
-  <si>
-    <t>categoria1</t>
-  </si>
-  <si>
-    <t>usuario2@example.com</t>
-  </si>
-  <si>
-    <t>Produto B</t>
-  </si>
-  <si>
-    <t>categoria2</t>
-  </si>
-  <si>
-    <t>usuario3@example.com</t>
-  </si>
-  <si>
-    <t>Produto C</t>
-  </si>
-  <si>
-    <t>categoria3</t>
-  </si>
-  <si>
-    <t>usuario4@example.com</t>
-  </si>
-  <si>
-    <t>Produto D</t>
-  </si>
-  <si>
-    <t>usuario5@example.com</t>
-  </si>
-  <si>
-    <t>Produto E</t>
-  </si>
-  <si>
-    <t>usuario6@example.com</t>
-  </si>
-  <si>
-    <t>Produto F</t>
-  </si>
-  <si>
-    <t>usuario7@example.com</t>
-  </si>
-  <si>
-    <t>Produto G</t>
-  </si>
-  <si>
-    <t>usuario8@example.com</t>
-  </si>
-  <si>
-    <t>Produto H</t>
-  </si>
-  <si>
-    <t>usuario9@example.com</t>
-  </si>
-  <si>
-    <t>Produto I</t>
-  </si>
-  <si>
-    <t>usuario10@example.com</t>
-  </si>
-  <si>
-    <t>Produto J</t>
-  </si>
-  <si>
-    <t>usuario11@example.com</t>
-  </si>
-  <si>
-    <t>Produto K</t>
-  </si>
-  <si>
-    <t>usuario12@example.com</t>
-  </si>
-  <si>
-    <t>Produto L</t>
-  </si>
-  <si>
-    <t>usuario13@example.com</t>
-  </si>
-  <si>
-    <t>Produto M</t>
-  </si>
-  <si>
-    <t>usuario14@example.com</t>
-  </si>
-  <si>
-    <t>Produto N</t>
-  </si>
-  <si>
-    <t>usuario15@example.com</t>
-  </si>
-  <si>
-    <t>Produto O</t>
-  </si>
-  <si>
-    <t>usuario16@example.com</t>
-  </si>
-  <si>
-    <t>Produto P</t>
-  </si>
-  <si>
-    <t>usuario17@example.com</t>
-  </si>
-  <si>
-    <t>Produto Q</t>
-  </si>
-  <si>
-    <t>usuario18@example.com</t>
-  </si>
-  <si>
-    <t>Produto R</t>
-  </si>
-  <si>
-    <t>usuario19@example.com</t>
-  </si>
-  <si>
-    <t>Produto S</t>
-  </si>
-  <si>
-    <t>usuario20@example.com</t>
-  </si>
-  <si>
-    <t>Produto T</t>
+    <t>Product A</t>
+  </si>
+  <si>
+    <t>category1</t>
+  </si>
+  <si>
+    <t>user2@example.com</t>
+  </si>
+  <si>
+    <t>Product B</t>
+  </si>
+  <si>
+    <t>category2</t>
+  </si>
+  <si>
+    <t>user3@example.com</t>
+  </si>
+  <si>
+    <t>Product C</t>
+  </si>
+  <si>
+    <t>category3</t>
+  </si>
+  <si>
+    <t>user4@example.com</t>
+  </si>
+  <si>
+    <t>Product D</t>
+  </si>
+  <si>
+    <t>user5@example.com</t>
+  </si>
+  <si>
+    <t>Product E</t>
+  </si>
+  <si>
+    <t>user6@example.com</t>
+  </si>
+  <si>
+    <t>Product F</t>
+  </si>
+  <si>
+    <t>user7@example.com</t>
+  </si>
+  <si>
+    <t>Product G</t>
+  </si>
+  <si>
+    <t>user8@example.com</t>
+  </si>
+  <si>
+    <t>Product H</t>
+  </si>
+  <si>
+    <t>user9@example.com</t>
+  </si>
+  <si>
+    <t>Product I</t>
+  </si>
+  <si>
+    <t>user10@example.com</t>
+  </si>
+  <si>
+    <t>Product J</t>
+  </si>
+  <si>
+    <t>user11@example.com</t>
+  </si>
+  <si>
+    <t>Product K</t>
+  </si>
+  <si>
+    <t>user12@example.com</t>
+  </si>
+  <si>
+    <t>Product L</t>
+  </si>
+  <si>
+    <t>user13@example.com</t>
+  </si>
+  <si>
+    <t>Product M</t>
+  </si>
+  <si>
+    <t>user14@example.com</t>
+  </si>
+  <si>
+    <t>user15@example.com</t>
+  </si>
+  <si>
+    <t>Product O</t>
+  </si>
+  <si>
+    <t>user16@example.com</t>
+  </si>
+  <si>
+    <t>Product P</t>
+  </si>
+  <si>
+    <t>user17@example.com</t>
+  </si>
+  <si>
+    <t>Product Q</t>
+  </si>
+  <si>
+    <t>user18@example.com</t>
+  </si>
+  <si>
+    <t>Product R</t>
+  </si>
+  <si>
+    <t>user19@example.com</t>
+  </si>
+  <si>
+    <t>Product S</t>
+  </si>
+  <si>
+    <t>user20@example.com</t>
+  </si>
+  <si>
+    <t>Product T</t>
   </si>
 </sst>
 </file>
@@ -179,7 +176,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -212,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -226,14 +223,17 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -555,12 +555,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -711,7 +711,7 @@
         <v>44933</v>
       </c>
       <c r="C8" s="7">
-        <v>-300</v>
+        <v>300</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
@@ -853,8 +853,8 @@
       <c r="C15" s="6">
         <v>309.99</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>36</v>
+      <c r="D15" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="E15" s="7">
         <v>2</v>
@@ -865,7 +865,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2">
         <v>44941</v>
@@ -874,7 +874,7 @@
         <v>399</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
@@ -885,7 +885,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2">
         <v>44942</v>
@@ -894,7 +894,7 @@
         <v>129</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="7">
         <v>5</v>
@@ -905,7 +905,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2">
         <v>44943</v>
@@ -914,7 +914,7 @@
         <v>159.99</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="7">
         <v>2</v>
@@ -925,7 +925,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2">
         <v>44944</v>
@@ -934,7 +934,7 @@
         <v>289.95</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="7">
         <v>3</v>
@@ -945,7 +945,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2">
         <v>44945</v>
@@ -954,7 +954,7 @@
         <v>349.9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="7">
         <v>4</v>
@@ -965,7 +965,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2">
         <v>44946</v>
@@ -974,7 +974,7 @@
         <v>399.99</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
chore: update excel data
</commit_message>
<xml_diff>
--- a/data/wrong.xlsx
+++ b/data/wrong.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>email</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>category</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Product A</t>
@@ -209,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -223,8 +220,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -232,14 +229,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -555,12 +549,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="26.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -584,9 +578,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="5"/>
       <c r="B2" s="2">
         <v>44927</v>
       </c>
@@ -594,18 +586,18 @@
         <v>150.5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="7">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>44928</v>
@@ -614,18 +606,18 @@
         <v>200</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="7">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>44929</v>
@@ -634,18 +626,18 @@
         <v>350.75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>44930</v>
@@ -654,18 +646,18 @@
         <v>99.99</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="7">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>44931</v>
@@ -674,18 +666,18 @@
         <v>499.99</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="7">
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>44932</v>
@@ -694,38 +686,38 @@
         <v>249</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>44933</v>
       </c>
       <c r="C8" s="7">
-        <v>300</v>
+        <v>-50</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="7">
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
         <v>44934</v>
@@ -734,18 +726,18 @@
         <v>450.5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
         <v>44935</v>
@@ -754,18 +746,18 @@
         <v>129.95</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="7">
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2">
         <v>44936</v>
@@ -774,18 +766,18 @@
         <v>89.9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="7">
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2">
         <v>44937</v>
@@ -794,18 +786,18 @@
         <v>199.9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2">
         <v>44938</v>
@@ -814,18 +806,18 @@
         <v>149.5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="7">
         <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
         <v>44939</v>
@@ -834,18 +826,18 @@
         <v>229</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="7">
         <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2">
         <v>44940</v>
@@ -853,19 +845,17 @@
       <c r="C15" s="6">
         <v>309.99</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="7">
         <v>2</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="2">
         <v>44941</v>
@@ -874,18 +864,18 @@
         <v>399</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2">
         <v>44942</v>
@@ -894,18 +884,18 @@
         <v>129</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="7">
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2">
         <v>44943</v>
@@ -914,18 +904,18 @@
         <v>159.99</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="7">
         <v>2</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2">
         <v>44944</v>
@@ -934,18 +924,18 @@
         <v>289.95</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="7">
         <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2">
         <v>44945</v>
@@ -954,18 +944,18 @@
         <v>349.9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="7">
         <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2">
         <v>44946</v>
@@ -974,13 +964,13 @@
         <v>399.99</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="7">
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>